<commit_message>
Lab 11a on SSE done
</commit_message>
<xml_diff>
--- a/Photonics_Labs/7_sem/Laser Gyroscope/Брославец.xlsx
+++ b/Photonics_Labs/7_sem/Laser Gyroscope/Брославец.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b566d95faa460c8a/Рабочий стол/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b566d95faa460c8a/GitHub/Labs/Photonics_Labs/7_sem/Laser Gyroscope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{340584EA-EC89-4FCB-BD1C-D8BD7D7EDDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08FF539F-5BF7-46F7-AE54-8F875235C698}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{340584EA-EC89-4FCB-BD1C-D8BD7D7EDDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3A5F621-AF12-45F5-B73C-39BD08F6DE50}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{1CA3D378-9E32-4109-BFAC-960507768EA5}"/>
   </bookViews>
@@ -28,10 +28,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,7 +368,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5FB3-4FAB-80E0-F10156AF8FA9}"/>
+              <c16:uniqueId val="{00000000-09E4-474C-A7F5-0EE47BC1F259}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -384,11 +380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="609387471"/>
-        <c:axId val="731228223"/>
+        <c:axId val="704097888"/>
+        <c:axId val="406712208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="609387471"/>
+        <c:axId val="704097888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,12 +441,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="731228223"/>
+        <c:crossAx val="406712208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="731228223"/>
+        <c:axId val="406712208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +503,480 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609387471"/>
+        <c:crossAx val="704097888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$2:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-1762.8809523809525</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1542.1428571428571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1409.0952380952383</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1221.6190476190477</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1038.6785714285716</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-751.41666666666674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-613.83333333333337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-706.05952380952385</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-672.79761904761915</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-636.51190476190482</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-576.03571428571433</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-542.77380952380952</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-497.41666666666674</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-495.90476190476193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-485.32142857142861</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2159</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1765.9047619047619</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1533.0714285714289</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1304.7738095238099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1118.8095238095239</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>952.50000000000011</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>802.82142857142856</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>648.60714285714289</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>588.13095238095241</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>553.35714285714289</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>514.04761904761904</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>498.92857142857144</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>464.15476190476193</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>579.05952380952385</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>497.41666666666674</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>450.54761904761909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$D$2:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>-1720</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1490</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1330</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1123</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-895</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-508</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-285</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-462</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-415</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-380</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-262</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-142</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-170</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-152</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2159</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1503</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1240</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>815</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-746C-4A1C-A8E1-61B77B5BF945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="398736304"/>
+        <c:axId val="396584416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="398736304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396584416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="396584416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398736304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -603,6 +1072,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1119,27 +1628,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>30956</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>351256</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>32843</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
+        <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD3D7FB3-CF13-4B1A-A2B2-484E08A25EB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713CE8BD-7BB0-421E-834D-C73D8BD966C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,6 +2177,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26192</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>169068</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F357C32-CB52-4C07-B4F5-8FCE68103F20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1457,268 +2518,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2100C9-70FE-4390-810E-47AA305B5D83}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V56" sqref="V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>-14.92</v>
       </c>
       <c r="B1">
         <v>-2265</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1">
+        <f>A1*$A$34</f>
+        <v>-2255.761904761905</v>
+      </c>
+      <c r="D1">
+        <f>B1</f>
+        <v>-2265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>-11.66</v>
       </c>
       <c r="B2">
         <v>-1720</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <f t="shared" ref="C2:C32" si="0">A2*$A$34</f>
+        <v>-1762.8809523809525</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D32" si="1">B2</f>
+        <v>-1720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>-10.199999999999999</v>
       </c>
       <c r="B3">
         <v>-1490</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>-1542.1428571428571</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>-1490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>-9.32</v>
       </c>
       <c r="B4">
         <v>-1330</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>-1409.0952380952383</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>-1330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>-8.08</v>
       </c>
       <c r="B5">
         <v>-1123</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-1221.6190476190477</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>-1123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>-6.87</v>
       </c>
       <c r="B6">
         <v>-895</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-1038.6785714285716</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-895</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>-4.97</v>
       </c>
       <c r="B7">
         <v>-508</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-751.41666666666674</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>-508</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>-4.0599999999999996</v>
       </c>
       <c r="B8">
         <v>-285</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-613.83333333333337</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>-4.67</v>
       </c>
       <c r="B9">
         <v>-462</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-706.05952380952385</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>-4.45</v>
       </c>
       <c r="B10">
         <v>-415</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-672.79761904761915</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>-415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>-4.21</v>
       </c>
       <c r="B11">
         <v>-380</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-636.51190476190482</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>-380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>-3.81</v>
       </c>
       <c r="B12">
         <v>-262</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-576.03571428571433</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>-262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>-3.59</v>
       </c>
       <c r="B13">
         <v>-207</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-542.77380952380952</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>-3.29</v>
       </c>
       <c r="B14">
         <v>-142</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-497.41666666666674</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>-3.28</v>
       </c>
       <c r="B15">
         <v>-170</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-495.90476190476193</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>-3.21</v>
       </c>
       <c r="B16">
         <v>-152</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-485.32142857142861</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>14.28</v>
       </c>
       <c r="B17">
         <v>2159</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2159</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>11.68</v>
       </c>
       <c r="B18">
         <v>1740</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1765.9047619047619</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>10.14</v>
       </c>
       <c r="B19">
         <v>1503</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1533.0714285714289</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>8.6300000000000008</v>
       </c>
       <c r="B20">
         <v>1240</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1304.7738095238099</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>7.4</v>
       </c>
       <c r="B21">
         <v>1015</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1118.8095238095239</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>6.3</v>
       </c>
       <c r="B22">
         <v>815</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>952.50000000000011</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>815</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>5.31</v>
       </c>
       <c r="B23">
         <v>638</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>802.82142857142856</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>4.29</v>
       </c>
       <c r="B24">
         <v>408</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>648.60714285714289</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3.89</v>
       </c>
       <c r="B25">
         <v>315</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>588.13095238095241</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3.66</v>
       </c>
       <c r="B26">
         <v>286</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>553.35714285714289</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>3.4</v>
       </c>
       <c r="B27">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>514.04761904761904</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>3.3</v>
       </c>
       <c r="B28">
         <v>202</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>498.92857142857144</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>3.07</v>
       </c>
       <c r="B29">
         <v>166</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>464.15476190476193</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>3.83</v>
       </c>
       <c r="B30">
         <v>339</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>579.05952380952385</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3.29</v>
       </c>
       <c r="B31">
         <v>200</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>497.41666666666674</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2.98</v>
       </c>
       <c r="B32">
         <v>166</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>450.54761904761909</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <f>B17/A17</f>
+        <v>151.1904761904762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>